<commit_message>
update: adicionado backlog feito
</commit_message>
<xml_diff>
--- a/BacklogAtual.xlsx
+++ b/BacklogAtual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gabriel\Dev\Faculdade\PI\SPRINT2\ARQUIVOS_GRUPO_ATUAL\Grupo-Tarefas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D65AB505-E4BC-4B5D-8392-9B1C929D27E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3576965-C4F6-46D9-B106-213C7B5A0734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C234F7D0-C0E1-43D8-8BDE-144E57B26FE3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>PROJETO ECLIPSEED - BACKLOG</t>
   </si>
@@ -115,14 +115,142 @@
     <t>IMPORTANTE</t>
   </si>
   <si>
-    <t>TERMINAR</t>
+    <t>Planilha de Riscos</t>
+  </si>
+  <si>
+    <t>Criar uma planilha que possui os riscos do projeto e na 
+construção dele para desta forma ter um melhor planejamento.</t>
+  </si>
+  <si>
+    <t>SP2</t>
+  </si>
+  <si>
+    <t>Especificação da 
+Dashboard</t>
+  </si>
+  <si>
+    <t>Especificar o uso da dashboard e como iremos utiliza-la.</t>
+  </si>
+  <si>
+    <t>Tela Inicial</t>
+  </si>
+  <si>
+    <t>Criar a tela inicial do site institucional seguindo o protótipo
+criado anteriormente.</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro</t>
+  </si>
+  <si>
+    <t>Criar a tela de cadastro e login (localmente) seguindo o
+protótipo criado anteriormente.</t>
+  </si>
+  <si>
+    <t>Integrar Dashboard
+Estático</t>
+  </si>
+  <si>
+    <t>Integrar o dashboard estático com o site institucional em 
+conjunto da ferramenta ChartJS.</t>
+  </si>
+  <si>
+    <t>Arquitetura Técnica</t>
+  </si>
+  <si>
+    <t>Criar uma arquitetura técnica do projeto falando sobre 
+a arquitetura utilizada na construção do mesmo.</t>
+  </si>
+  <si>
+    <t>Melhorar o Banco de 
+Dados</t>
+  </si>
+  <si>
+    <t>Melhorar as tabelas criadas anteriormente seguindo o 
+contexto do projeto.</t>
+  </si>
+  <si>
+    <t>Modelagem lógica</t>
+  </si>
+  <si>
+    <t>Criar a modelagem/diagrama lógica das tabelas criadas
+no banco de dados e seu tipo de relação com outras tabelas.</t>
+  </si>
+  <si>
+    <t>Integrar o sensor utilizado (LDR) com os gráficos fornecidos
+através da API dat-aqu-ino e verificar seu correto funcionamento</t>
+  </si>
+  <si>
+    <t>Sensor + Gráficos + API</t>
+  </si>
+  <si>
+    <t>MySQL na VM</t>
+  </si>
+  <si>
+    <t>Instalar e configurar o MySQL na Máquina Virtual e inserir
+dados da tabela criada anteriormente nele, além de verificar seu correto funcionamento</t>
+  </si>
+  <si>
+    <t>Integração do Arduino
+com o Banco de Dados da VM</t>
+  </si>
+  <si>
+    <t>Integrar o arduino/sensor com o banco de dados estruturado
+na máquina virtual através da utilização da API.</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>Integrar o Site Institucional
+com o Banco de Dados da VM</t>
+  </si>
+  <si>
+    <t>Integrar o site institucional com o banco de dados da VM para
+desta forma ele conseguir fornecer os dados para o cliente sobre
+a luminosidade coletada pelo sensor, além de conseguir realizar
+o cadastro do usuário e o login.</t>
+  </si>
+  <si>
+    <t>Hospedar o Site 
+Intitucional na VM</t>
+  </si>
+  <si>
+    <t>Colocar o site institucional na Máquina Virtual, visto que até
+o momento ele estava hospedado no Windows.</t>
+  </si>
+  <si>
+    <t>Fluxograma do Suporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação da 
+Ferramenta HelpDesk 
+</t>
+  </si>
+  <si>
+    <t>Interface Intuitiva</t>
+  </si>
+  <si>
+    <t>DESEJÁVEL</t>
+  </si>
+  <si>
+    <t>Criar  uma representação visual que detalha as etapas e 
+processos do atendimento ao cliente, desde o primeiro 
+contato até a resolução.</t>
+  </si>
+  <si>
+    <t>Implementar um software ou sistema que centraliza e 
+organiza o atendimento ao cliente para assim ter um melhor
+gerenciamento.</t>
+  </si>
+  <si>
+    <t>Fazer o site institucional ter uma interface intuitiva.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +268,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -233,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,13 +388,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F705186-7EB0-469F-BE70-E045BA0AA36B}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,19 +798,19 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -669,13 +821,13 @@
       <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -686,30 +838,30 @@
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -720,79 +872,357 @@
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="B9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>